<commit_message>
Scrum documentation added , and Timesheet.md created
</commit_message>
<xml_diff>
--- a/2.2_P.CoB_Time_registration_for10.xlsx
+++ b/2.2_P.CoB_Time_registration_for10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Courses\2.2 Project Client on Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tavarista\Desktop\uni\2 YEAR\Client ob Board (Or1on)\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E655F07E-9948-4291-B9E2-F505DEA8BB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4CC66A-B600-4CE0-A527-EDE50352A7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,12 +44,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
-  <si>
-    <t>Student-1</t>
-  </si>
-  <si>
-    <t>Student-2</t>
-  </si>
   <si>
     <t>Student-3</t>
   </si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>Student-</t>
+  </si>
+  <si>
+    <t>Rafael Tavares</t>
   </si>
 </sst>
 </file>
@@ -654,6 +654,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -666,12 +667,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -681,7 +676,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +756,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Student-1</c:v>
+                  <c:v>Rafael Tavares</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -842,7 +842,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Student-2</c:v>
+                  <c:v>Student-</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1746,7 +1746,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1987,7 +1987,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="82118767"/>
@@ -2046,7 +2046,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="82118351"/>
@@ -2088,7 +2088,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2122,7 +2122,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3066,49 +3066,49 @@
   <sheetData>
     <row r="1" spans="1:8" s="28" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="45" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="45" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="36" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3390,32 +3390,32 @@
         <f>Total!$L$1</f>
         <v>Week 8</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="str">
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -3563,18 +3563,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -3714,16 +3714,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -3863,16 +3863,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -4012,16 +4012,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -4059,7 +4059,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -4163,16 +4163,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -4210,7 +4210,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -4314,16 +4314,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -4361,7 +4361,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -4465,16 +4465,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -4512,7 +4512,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -4616,16 +4616,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -4663,7 +4663,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -4767,16 +4767,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -4814,7 +4814,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -4915,17 +4915,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4936,8 +4936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5139,50 +5139,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="D1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="D1" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>35</v>
-      </c>
       <c r="D2" s="17" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3">
         <f>'Week (1)'!$H$11</f>
@@ -5222,10 +5222,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
       <c r="D3" s="17" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3">
         <f>'Week (1)'!$H$21</f>
@@ -5265,14 +5265,14 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>36</v>
-      </c>
       <c r="D4" s="17" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
         <f>'Week (1)'!$H$30</f>
@@ -5312,10 +5312,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
       <c r="D5" s="17" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="3">
         <f>'Week (1)'!$H$39</f>
@@ -5358,7 +5358,7 @@
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="D6" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3">
         <f>'Week (1)'!$H$48</f>
@@ -5401,7 +5401,7 @@
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
       <c r="D7" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3">
         <f>'Week (1)'!$H$57</f>
@@ -5444,7 +5444,7 @@
       <c r="A8" s="31"/>
       <c r="B8" s="32"/>
       <c r="D8" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3">
         <f>'Week (1)'!$H$66</f>
@@ -5487,7 +5487,7 @@
       <c r="A9" s="31"/>
       <c r="B9" s="32"/>
       <c r="D9" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3">
         <f>'Week (1)'!$H$75</f>
@@ -5530,7 +5530,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="32"/>
       <c r="D10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="3">
         <f>'Week (1)'!$H$84</f>
@@ -5573,7 +5573,7 @@
       <c r="A11" s="31"/>
       <c r="B11" s="32"/>
       <c r="D11" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3">
         <f>'Week (1)'!$H$93</f>
@@ -5616,38 +5616,38 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="D12" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="16">
-        <f>SUM(E2:E11)</f>
+        <f t="shared" ref="E12:L12" si="3">SUM(E2:E11)</f>
         <v>0</v>
       </c>
       <c r="F12" s="16">
-        <f>SUM(F2:F11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G12" s="16">
-        <f>SUM(G2:G11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H12" s="16">
-        <f>SUM(H2:H11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" s="16">
-        <f>SUM(I2:I11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J12" s="16">
-        <f>SUM(J2:J11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K12" s="16">
-        <f>SUM(K2:K11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="16">
-        <f>SUM(L2:L11)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5655,7 +5655,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="D13" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21">
@@ -5682,7 +5682,7 @@
       <c r="A14" s="33"/>
       <c r="B14" s="32"/>
       <c r="D14" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E14" s="19">
         <f>E15-E12</f>
@@ -5693,68 +5693,68 @@
         <v>960</v>
       </c>
       <c r="G14" s="19">
-        <f t="shared" ref="G14:L14" si="3">F14-G12</f>
+        <f t="shared" ref="G14:L14" si="4">F14-G12</f>
         <v>960</v>
       </c>
       <c r="H14" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
       <c r="I14" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
       <c r="J14" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
       <c r="K14" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
       <c r="L14" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
       <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="35">
         <f>COUNTIF(D2:D11, "&gt;''" )*12</f>
         <v>120</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="19">
-        <f t="shared" ref="E15:K15" si="4">$B$15+F15</f>
+        <f t="shared" ref="E15:K15" si="5">$B$15+F15</f>
         <v>960</v>
       </c>
       <c r="F15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>840</v>
       </c>
       <c r="G15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>720</v>
       </c>
       <c r="H15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>600</v>
       </c>
       <c r="I15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>480</v>
       </c>
       <c r="J15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>360</v>
       </c>
       <c r="K15" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="L15" s="19">
@@ -6055,52 +6055,52 @@
         <f>Total!$E$1</f>
         <v>Week 1</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="H4" s="8" t="str">
         <f>Total!$M$1</f>
@@ -6109,7 +6109,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -6231,18 +6231,18 @@
     <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B13" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B13" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="43"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
@@ -6280,7 +6280,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -6385,16 +6385,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B23" s="42" t="str">
+      <c r="B23" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
@@ -6432,7 +6432,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -6503,27 +6503,27 @@
         <v>Total</v>
       </c>
       <c r="B30" s="12">
-        <f>SUM(B25:B29)</f>
+        <f t="shared" ref="B30:G30" si="7">SUM(B25:B29)</f>
         <v>0</v>
       </c>
       <c r="C30" s="12">
-        <f>SUM(C25:C29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D30" s="12">
-        <f>SUM(D25:D29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E30" s="12">
-        <f>SUM(E25:E29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F30" s="12">
-        <f>SUM(F25:F29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G30" s="12">
-        <f>SUM(G25:G29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H30" s="12">
@@ -6536,16 +6536,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B32" s="42" t="str">
+      <c r="B32" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="44"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="43"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="str">
@@ -6557,33 +6557,33 @@
         <v>Ma</v>
       </c>
       <c r="C33" s="8" t="str">
-        <f t="shared" ref="C33:H33" si="7">C$4</f>
+        <f t="shared" ref="C33:H33" si="8">C$4</f>
         <v>Di</v>
       </c>
       <c r="D33" s="8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Wo</v>
       </c>
       <c r="E33" s="8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Do</v>
       </c>
       <c r="F33" s="8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Vr</v>
       </c>
       <c r="G33" s="8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Za/Zo</v>
       </c>
       <c r="H33" s="8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Total</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -6605,7 +6605,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="6">
-        <f t="shared" ref="H35:H38" si="8">SUM(B35:G35)</f>
+        <f t="shared" ref="H35:H38" si="9">SUM(B35:G35)</f>
         <v>0</v>
       </c>
     </row>
@@ -6618,7 +6618,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6631,7 +6631,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6644,7 +6644,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -6654,27 +6654,27 @@
         <v>Total</v>
       </c>
       <c r="B39" s="12">
-        <f>SUM(B34:B38)</f>
+        <f t="shared" ref="B39:G39" si="10">SUM(B34:B38)</f>
         <v>0</v>
       </c>
       <c r="C39" s="12">
-        <f>SUM(C34:C38)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D39" s="12">
-        <f>SUM(D34:D38)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E39" s="12">
-        <f>SUM(E34:E38)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F39" s="12">
-        <f>SUM(F34:F38)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G39" s="12">
-        <f>SUM(G34:G38)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H39" s="12">
@@ -6687,16 +6687,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B41" s="42" t="str">
+      <c r="B41" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="44"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="43"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="str">
@@ -6708,33 +6708,33 @@
         <v>Ma</v>
       </c>
       <c r="C42" s="8" t="str">
-        <f t="shared" ref="C42:H42" si="9">C$4</f>
+        <f t="shared" ref="C42:H42" si="11">C$4</f>
         <v>Di</v>
       </c>
       <c r="D42" s="8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Wo</v>
       </c>
       <c r="E42" s="8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Do</v>
       </c>
       <c r="F42" s="8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Vr</v>
       </c>
       <c r="G42" s="8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Za/Zo</v>
       </c>
       <c r="H42" s="8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Total</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -6756,7 +6756,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="6">
-        <f t="shared" ref="H44:H47" si="10">SUM(B44:G44)</f>
+        <f t="shared" ref="H44:H47" si="12">SUM(B44:G44)</f>
         <v>0</v>
       </c>
     </row>
@@ -6769,7 +6769,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6782,7 +6782,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6795,7 +6795,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6805,27 +6805,27 @@
         <v>Total</v>
       </c>
       <c r="B48" s="12">
-        <f t="shared" ref="B48:G48" si="11">SUM(B43:B47)</f>
+        <f t="shared" ref="B48:G48" si="13">SUM(B43:B47)</f>
         <v>0</v>
       </c>
       <c r="C48" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D48" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E48" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F48" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G48" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H48" s="12">
@@ -6838,16 +6838,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B50" s="42" t="str">
+      <c r="B50" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="44"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="43"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="str">
@@ -6859,33 +6859,33 @@
         <v>Ma</v>
       </c>
       <c r="C51" s="8" t="str">
-        <f t="shared" ref="C51:H51" si="12">C$4</f>
+        <f t="shared" ref="C51:H51" si="14">C$4</f>
         <v>Di</v>
       </c>
       <c r="D51" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Wo</v>
       </c>
       <c r="E51" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Do</v>
       </c>
       <c r="F51" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Vr</v>
       </c>
       <c r="G51" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Za/Zo</v>
       </c>
       <c r="H51" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>Total</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -6907,7 +6907,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="6">
-        <f t="shared" ref="H53:H56" si="13">SUM(B53:G53)</f>
+        <f t="shared" ref="H53:H56" si="15">SUM(B53:G53)</f>
         <v>0</v>
       </c>
     </row>
@@ -6920,7 +6920,7 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6933,7 +6933,7 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6946,7 +6946,7 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -6956,27 +6956,27 @@
         <v>Total</v>
       </c>
       <c r="B57" s="12">
-        <f t="shared" ref="B57:G57" si="14">SUM(B52:B56)</f>
+        <f t="shared" ref="B57:G57" si="16">SUM(B52:B56)</f>
         <v>0</v>
       </c>
       <c r="C57" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="D57" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E57" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F57" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G57" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H57" s="12">
@@ -6989,16 +6989,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B59" s="42" t="str">
+      <c r="B59" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="44"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="43"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="str">
@@ -7010,33 +7010,33 @@
         <v>Ma</v>
       </c>
       <c r="C60" s="8" t="str">
-        <f t="shared" ref="C60:H60" si="15">C$4</f>
+        <f t="shared" ref="C60:H60" si="17">C$4</f>
         <v>Di</v>
       </c>
       <c r="D60" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>Wo</v>
       </c>
       <c r="E60" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>Do</v>
       </c>
       <c r="F60" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>Vr</v>
       </c>
       <c r="G60" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>Za/Zo</v>
       </c>
       <c r="H60" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>Total</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -7058,7 +7058,7 @@
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
       <c r="H62" s="6">
-        <f t="shared" ref="H62:H65" si="16">SUM(B62:G62)</f>
+        <f t="shared" ref="H62:H65" si="18">SUM(B62:G62)</f>
         <v>0</v>
       </c>
     </row>
@@ -7071,7 +7071,7 @@
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -7084,7 +7084,7 @@
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -7097,7 +7097,7 @@
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
       <c r="H65" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -7107,27 +7107,27 @@
         <v>Total</v>
       </c>
       <c r="B66" s="12">
-        <f t="shared" ref="B66:G66" si="17">SUM(B61:B65)</f>
+        <f t="shared" ref="B66:G66" si="19">SUM(B61:B65)</f>
         <v>0</v>
       </c>
       <c r="C66" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="D66" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E66" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F66" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G66" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H66" s="12">
@@ -7140,16 +7140,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B68" s="42" t="str">
+      <c r="B68" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="44"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="43"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="str">
@@ -7161,33 +7161,33 @@
         <v>Ma</v>
       </c>
       <c r="C69" s="8" t="str">
-        <f t="shared" ref="C69:H69" si="18">C$4</f>
+        <f t="shared" ref="C69:H69" si="20">C$4</f>
         <v>Di</v>
       </c>
       <c r="D69" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Wo</v>
       </c>
       <c r="E69" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Do</v>
       </c>
       <c r="F69" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Vr</v>
       </c>
       <c r="G69" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Za/Zo</v>
       </c>
       <c r="H69" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>Total</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -7209,7 +7209,7 @@
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
       <c r="H71" s="6">
-        <f t="shared" ref="H71:H74" si="19">SUM(B71:G71)</f>
+        <f t="shared" ref="H71:H74" si="21">SUM(B71:G71)</f>
         <v>0</v>
       </c>
     </row>
@@ -7222,7 +7222,7 @@
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
       <c r="H72" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7235,7 +7235,7 @@
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
       <c r="H73" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7248,7 +7248,7 @@
       <c r="F74" s="10"/>
       <c r="G74" s="10"/>
       <c r="H74" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7258,27 +7258,27 @@
         <v>Total</v>
       </c>
       <c r="B75" s="12">
-        <f t="shared" ref="B75:G75" si="20">SUM(B70:B74)</f>
+        <f t="shared" ref="B75:G75" si="22">SUM(B70:B74)</f>
         <v>0</v>
       </c>
       <c r="C75" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="D75" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="E75" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F75" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G75" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H75" s="12">
@@ -7291,16 +7291,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B77" s="42" t="str">
+      <c r="B77" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="44"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
+      <c r="H77" s="43"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="str">
@@ -7312,33 +7312,33 @@
         <v>Ma</v>
       </c>
       <c r="C78" s="8" t="str">
-        <f t="shared" ref="C78:H78" si="21">C$4</f>
+        <f t="shared" ref="C78:H78" si="23">C$4</f>
         <v>Di</v>
       </c>
       <c r="D78" s="8" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>Wo</v>
       </c>
       <c r="E78" s="8" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>Do</v>
       </c>
       <c r="F78" s="8" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>Vr</v>
       </c>
       <c r="G78" s="8" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>Za/Zo</v>
       </c>
       <c r="H78" s="8" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>Total</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -7360,7 +7360,7 @@
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
       <c r="H80" s="6">
-        <f t="shared" ref="H80:H83" si="22">SUM(B80:G80)</f>
+        <f t="shared" ref="H80:H83" si="24">SUM(B80:G80)</f>
         <v>0</v>
       </c>
     </row>
@@ -7373,7 +7373,7 @@
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
       <c r="H81" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -7386,7 +7386,7 @@
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
       <c r="H82" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -7399,7 +7399,7 @@
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
       <c r="H83" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -7409,27 +7409,27 @@
         <v>Total</v>
       </c>
       <c r="B84" s="12">
-        <f t="shared" ref="B84:G84" si="23">SUM(B79:B83)</f>
+        <f t="shared" ref="B84:G84" si="25">SUM(B79:B83)</f>
         <v>0</v>
       </c>
       <c r="C84" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="D84" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="E84" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="F84" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G84" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="H84" s="12">
@@ -7442,16 +7442,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B86" s="42" t="str">
+      <c r="B86" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C86" s="43"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
-      <c r="G86" s="43"/>
-      <c r="H86" s="44"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="42"/>
+      <c r="H86" s="43"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="str">
@@ -7463,33 +7463,33 @@
         <v>Ma</v>
       </c>
       <c r="C87" s="8" t="str">
-        <f t="shared" ref="C87:H87" si="24">C$4</f>
+        <f t="shared" ref="C87:H87" si="26">C$4</f>
         <v>Di</v>
       </c>
       <c r="D87" s="8" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>Wo</v>
       </c>
       <c r="E87" s="8" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>Do</v>
       </c>
       <c r="F87" s="8" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>Vr</v>
       </c>
       <c r="G87" s="8" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>Za/Zo</v>
       </c>
       <c r="H87" s="8" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>Total</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -7511,7 +7511,7 @@
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
       <c r="H89" s="6">
-        <f t="shared" ref="H89:H92" si="25">SUM(B89:G89)</f>
+        <f t="shared" ref="H89:H92" si="27">SUM(B89:G89)</f>
         <v>0</v>
       </c>
     </row>
@@ -7524,7 +7524,7 @@
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
       <c r="H90" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -7537,7 +7537,7 @@
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
       <c r="H91" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -7550,7 +7550,7 @@
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
       <c r="H92" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -7560,27 +7560,27 @@
         <v>Total</v>
       </c>
       <c r="B93" s="12">
-        <f t="shared" ref="B93:G93" si="26">SUM(B88:B92)</f>
+        <f t="shared" ref="B93:G93" si="28">SUM(B88:B92)</f>
         <v>0</v>
       </c>
       <c r="C93" s="12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="D93" s="12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E93" s="12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="F93" s="12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G93" s="12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H93" s="12">
@@ -7590,17 +7590,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="B86:H86"/>
     <mergeCell ref="B41:H41"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B59:H59"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7885,32 +7885,32 @@
         <f>Total!$F$1</f>
         <v>Week 2</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="str">
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -8058,18 +8058,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -8209,16 +8209,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -8358,16 +8358,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -8507,16 +8507,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -8554,7 +8554,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -8658,16 +8658,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -8705,7 +8705,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -8809,16 +8809,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -8856,7 +8856,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -8960,16 +8960,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -9007,7 +9007,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -9111,16 +9111,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -9158,7 +9158,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -9262,16 +9262,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -9309,7 +9309,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -9410,17 +9410,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9700,32 +9700,32 @@
         <f>Total!$G$1</f>
         <v>Week 3</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="str">
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -9873,18 +9873,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -10024,16 +10024,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -10173,16 +10173,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -10322,16 +10322,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -10369,7 +10369,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -10473,16 +10473,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -10520,7 +10520,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -10624,16 +10624,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -10671,7 +10671,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -10775,16 +10775,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -10822,7 +10822,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -10926,16 +10926,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -10973,7 +10973,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -11077,16 +11077,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -11124,7 +11124,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -11225,17 +11225,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11515,32 +11515,32 @@
         <f>Total!$H$1</f>
         <v>Week 4</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="str">
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -11688,18 +11688,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -11839,16 +11839,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -11988,16 +11988,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -12137,16 +12137,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -12184,7 +12184,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -12288,16 +12288,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -12335,7 +12335,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -12439,16 +12439,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -12486,7 +12486,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -12590,16 +12590,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -12637,7 +12637,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -12741,16 +12741,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -12788,7 +12788,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -12892,16 +12892,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -12939,7 +12939,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -13040,17 +13040,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13330,31 +13330,31 @@
         <f>Total!$I$1</f>
         <v>Week 5</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -13502,18 +13502,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -13653,16 +13653,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -13802,16 +13802,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -13951,16 +13951,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -13998,7 +13998,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -14102,16 +14102,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -14149,7 +14149,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -14253,16 +14253,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -14300,7 +14300,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -14404,16 +14404,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -14451,7 +14451,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -14555,16 +14555,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -14602,7 +14602,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -14706,16 +14706,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -14753,7 +14753,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -14854,17 +14854,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15144,32 +15144,32 @@
         <f>Total!$J$1</f>
         <v>Week 6</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="str">
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -15317,18 +15317,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -15468,16 +15468,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -15617,16 +15617,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -15766,16 +15766,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -15810,7 +15810,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -15914,16 +15914,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -15961,7 +15961,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -16065,16 +16065,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -16112,7 +16112,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -16216,16 +16216,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -16263,7 +16263,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -16367,16 +16367,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -16414,7 +16414,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -16518,16 +16518,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -16565,7 +16565,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -16666,17 +16666,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16956,32 +16956,32 @@
         <f>Total!$K$1</f>
         <v>Week 7</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="44" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>Total!D2</f>
-        <v>Student-1</v>
-      </c>
-      <c r="B3" s="42" t="str">
+        <v>Rafael Tavares</v>
+      </c>
+      <c r="B3" s="41" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -17129,18 +17129,18 @@
     <row r="12" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>Total!D3</f>
-        <v>Student-2</v>
-      </c>
-      <c r="B12" s="42" t="str">
+        <v>Student-</v>
+      </c>
+      <c r="B12" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -17280,16 +17280,16 @@
         <f>Total!D4</f>
         <v>Student-3</v>
       </c>
-      <c r="B21" s="42" t="str">
+      <c r="B21" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -17429,16 +17429,16 @@
         <f>Total!D5</f>
         <v>Student-4</v>
       </c>
-      <c r="B30" s="42" t="str">
+      <c r="B30" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -17578,16 +17578,16 @@
         <f>Total!D6</f>
         <v>Student-5</v>
       </c>
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -17625,7 +17625,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -17729,16 +17729,16 @@
         <f>Total!D7</f>
         <v>Student-6</v>
       </c>
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -17776,7 +17776,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -17880,16 +17880,16 @@
         <f>Total!D8</f>
         <v>Student-7</v>
       </c>
-      <c r="B57" s="42" t="str">
+      <c r="B57" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="44"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -17927,7 +17927,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -18031,16 +18031,16 @@
         <f>Total!D9</f>
         <v>Student-8</v>
       </c>
-      <c r="B66" s="42" t="str">
+      <c r="B66" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="44"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -18078,7 +18078,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -18182,16 +18182,16 @@
         <f>Total!D10</f>
         <v>Student-9</v>
       </c>
-      <c r="B75" s="42" t="str">
+      <c r="B75" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="44"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -18229,7 +18229,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -18333,16 +18333,16 @@
         <f>Total!D11</f>
         <v>Student-10</v>
       </c>
-      <c r="B84" s="42" t="str">
+      <c r="B84" s="41" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="44"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -18380,7 +18380,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -18481,17 +18481,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18499,6 +18499,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c6664f9864b54a78bdf9e6230de1c78b>
+    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100294690D6A57C3C4B8650464765815F1C" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="bf1d2ff51e740e451b46e7c13bf9e6da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45f6ce90-ba85-4ef2-b43f-c64448cd95eb" xmlns:ns3="c7549584-aa9c-449c-abfe-2ca02f3a7188" xmlns:ns4="6c73e52c-07d4-4617-ab67-464747257e8d" xmlns:ns5="ab37b2fe-4f81-426e-b942-40459dbac68c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8575fd65d7959dd12bd4dc11d36e634e" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="45f6ce90-ba85-4ef2-b43f-c64448cd95eb"/>
@@ -18741,27 +18761,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c6664f9864b54a78bdf9e6230de1c78b>
-    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
+    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{724CCB8E-5E6A-4B8C-A558-5D9223ADF390}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18780,23 +18799,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
-    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>